<commit_message>
add  torch tensor samples
</commit_message>
<xml_diff>
--- a/data/regression1.xlsx
+++ b/data/regression1.xlsx
@@ -8,76 +8,76 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\software\python-training-workspace\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EBC4B81-57F7-40C0-9E09-1706D65D7F70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D59C5285-2AF6-415D-8391-3ABE62E78A0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2085" yWindow="1740" windowWidth="21600" windowHeight="11385" xr2:uid="{3E6FC988-522D-40AE-8855-7C43750CD683}"/>
+    <workbookView xWindow="2085" yWindow="1740" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{3E6FC988-522D-40AE-8855-7C43750CD683}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
-    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
+    <sheet name="Tabelle3" sheetId="3" r:id="rId2"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">Tabelle1!$B$16:$B$17</definedName>
-    <definedName name="solver_adj" localSheetId="1" hidden="1">Tabelle2!$B$4:$B$6</definedName>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">Tabelle2!$B$4:$B$6</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
-    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="1" hidden="1">Tabelle2!$B$4:$B$6</definedName>
-    <definedName name="solver_lhs2" localSheetId="1" hidden="1">Tabelle2!$B$4:$B$6</definedName>
+    <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="2" hidden="1">Tabelle2!$B$4:$B$6</definedName>
+    <definedName name="solver_lhs2" localSheetId="2" hidden="1">Tabelle2!$B$4:$B$6</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
-    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
-    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_num" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_num" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">Tabelle1!$E$4</definedName>
-    <definedName name="solver_opt" localSheetId="1" hidden="1">Tabelle2!$G$4</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">Tabelle2!$G$4</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
-    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="1" hidden="1">4</definedName>
-    <definedName name="solver_rel2" localSheetId="1" hidden="1">3</definedName>
-    <definedName name="solver_rhs1" localSheetId="1" hidden="1">Ganzzahlig</definedName>
-    <definedName name="solver_rhs2" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="2" hidden="1">4</definedName>
+    <definedName name="solver_rel2" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rhs1" localSheetId="2" hidden="1">Ganzzahlig</definedName>
+    <definedName name="solver_rhs2" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
-    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
-    <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -96,8 +96,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>x</t>
   </si>
@@ -146,15 +168,22 @@
   <si>
     <t>Personen ges. für Transport</t>
   </si>
+  <si>
+    <t>y = mx + b</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,6 +198,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="17"/>
+      <color rgb="FF494B51"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -231,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -245,6 +280,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -677,7 +714,506 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle3!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>y</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle3!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle3!$B$2:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>122.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>133.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>180</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8F5C-425C-B157-F952BC8FE9EA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle3!$A$2:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle3!$G$2:$G$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>104.89090909090909</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>111.69272727272728</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>118.49454545454546</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>125.29636363636364</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>132.09818181818181</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>138.9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>145.7018181818182</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>152.50363636363636</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>159.30545454545455</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>166.10727272727274</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>172.90909090909093</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>179.71090909090913</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>186.51272727272732</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>193.31454545454545</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8F5C-425C-B157-F952BC8FE9EA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="745124376"/>
+        <c:axId val="745122736"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="745124376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="0.000000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="745122736"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="745122736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.000000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="745124376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1233,6 +1769,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1254,6 +2293,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B6AEB8F-F83A-4A17-A9DC-C0FBDD57056F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB125C8E-37B4-475E-8BEC-28D7EC5D1413}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1573,7 +2653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B589BB41-1C4A-450C-8230-DDB3BE7AA956}">
   <dimension ref="A3:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -1779,6 +2859,212 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C701F8BA-2E76-4B73-923C-0FE39CE90C73}">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.42578125" style="11"/>
+    <col min="4" max="4" width="22.85546875" style="11" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="21.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="12"/>
+      <c r="E1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11">
+        <v>100</v>
+      </c>
+      <c r="E2" s="11" cm="1">
+        <f t="array" ref="E2:F2">LINEST(B2:B12,A2:A12)</f>
+        <v>68.01818181818183</v>
+      </c>
+      <c r="F2" s="11">
+        <v>36.872727272727261</v>
+      </c>
+      <c r="G2" s="11">
+        <f>$E$2*A2+$F$2</f>
+        <v>104.89090909090909</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B3" s="11">
+        <v>122.3</v>
+      </c>
+      <c r="G3" s="11">
+        <f t="shared" ref="G3:G15" si="0">$E$2*A3+$F$2</f>
+        <v>111.69272727272728</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>1.2</v>
+      </c>
+      <c r="B4" s="11">
+        <v>110</v>
+      </c>
+      <c r="G4" s="11">
+        <f t="shared" si="0"/>
+        <v>118.49454545454546</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>1.3</v>
+      </c>
+      <c r="B5" s="11">
+        <v>130</v>
+      </c>
+      <c r="G5" s="11">
+        <f t="shared" si="0"/>
+        <v>125.29636363636364</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <v>1.4</v>
+      </c>
+      <c r="B6" s="11">
+        <v>133.6</v>
+      </c>
+      <c r="G6" s="11">
+        <f t="shared" si="0"/>
+        <v>132.09818181818181</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="B7" s="11">
+        <v>135</v>
+      </c>
+      <c r="G7" s="11">
+        <f t="shared" si="0"/>
+        <v>138.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>1.6</v>
+      </c>
+      <c r="B8" s="11">
+        <v>145</v>
+      </c>
+      <c r="G8" s="11">
+        <f t="shared" si="0"/>
+        <v>145.7018181818182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
+        <v>1.7</v>
+      </c>
+      <c r="B9" s="11">
+        <v>160</v>
+      </c>
+      <c r="G9" s="11">
+        <f t="shared" si="0"/>
+        <v>152.50363636363636</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
+        <v>1.8</v>
+      </c>
+      <c r="B10" s="11">
+        <v>152</v>
+      </c>
+      <c r="G10" s="11">
+        <f t="shared" si="0"/>
+        <v>159.30545454545455</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
+        <v>1.9</v>
+      </c>
+      <c r="B11" s="11">
+        <v>160</v>
+      </c>
+      <c r="G11" s="11">
+        <f t="shared" si="0"/>
+        <v>166.10727272727274</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
+        <v>2</v>
+      </c>
+      <c r="B12" s="11">
+        <v>180</v>
+      </c>
+      <c r="G12" s="11">
+        <f t="shared" si="0"/>
+        <v>172.90909090909093</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
+        <v>2.1</v>
+      </c>
+      <c r="G13" s="11">
+        <f t="shared" si="0"/>
+        <v>179.71090909090913</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="11">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G14" s="11">
+        <f t="shared" si="0"/>
+        <v>186.51272727272732</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="11">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G15" s="11">
+        <f t="shared" si="0"/>
+        <v>193.31454545454545</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0365B85-C27E-4212-A845-9180E7635ADF}">
   <dimension ref="A3:G7"/>
   <sheetViews>
@@ -1861,16 +3147,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C701F8BA-2E76-4B73-923C-0FE39CE90C73}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>